<commit_message>
ch ch ch changes
</commit_message>
<xml_diff>
--- a/divinity/Skills.xlsx
+++ b/divinity/Skills.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jturo\notes\divinity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08232550-7E44-459B-A665-14BE41A6CAFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1F1151-9552-42BC-9620-7FDA3DAF59A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{22CF8C86-0986-46F7-901E-B0479304723F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="146">
   <si>
     <t>Aerotheurge</t>
   </si>
@@ -609,6 +609,12 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{91EF0500-EACC-4F56-8167-B7EC3E2BB0C0}" name="brenda" displayName="brenda" ref="A1:D54" totalsRowShown="0">
   <autoFilter ref="A1:D54" xr:uid="{BF9C7B15-02F1-4DC6-B7CC-0ADE24FA67EF}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Man-At-Arms"/>
+        <filter val="Scoundrel"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>
@@ -1778,7 +1784,7 @@
       </c>
       <c r="D54">
         <f>IF(ISNA(VLOOKUP(A54,danger[],1,FALSE)),0,IF(VLOOKUP(A54,danger[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A54,brenda[],1,FALSE)),0,IF(VLOOKUP(A54,brenda[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A54,madora[],1,FALSE)),0,IF(VLOOKUP(A54,madora[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A54,jehan[],1,FALSE)),0,IF(VLOOKUP(A54,jehan[],4,FALSE)="",1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1943,7 +1949,7 @@
       </c>
       <c r="D65">
         <f>IF(ISNA(VLOOKUP(A65,danger[],1,FALSE)),0,IF(VLOOKUP(A65,danger[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A65,brenda[],1,FALSE)),0,IF(VLOOKUP(A65,brenda[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A65,madora[],1,FALSE)),0,IF(VLOOKUP(A65,madora[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A65,jehan[],1,FALSE)),0,IF(VLOOKUP(A65,jehan[],4,FALSE)="",1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -2693,7 +2699,7 @@
       </c>
       <c r="D115">
         <f>IF(ISNA(VLOOKUP(A115,danger[],1,FALSE)),0,IF(VLOOKUP(A115,danger[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A115,brenda[],1,FALSE)),0,IF(VLOOKUP(A115,brenda[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A115,madora[],1,FALSE)),0,IF(VLOOKUP(A115,madora[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A115,jehan[],1,FALSE)),0,IF(VLOOKUP(A115,jehan[],4,FALSE)="",1,0))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -2783,7 +2789,7 @@
       </c>
       <c r="D121">
         <f>IF(ISNA(VLOOKUP(A121,danger[],1,FALSE)),0,IF(VLOOKUP(A121,danger[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A121,brenda[],1,FALSE)),0,IF(VLOOKUP(A121,brenda[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A121,madora[],1,FALSE)),0,IF(VLOOKUP(A121,madora[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A121,jehan[],1,FALSE)),0,IF(VLOOKUP(A121,jehan[],4,FALSE)="",1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -2919,7 +2925,7 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3090,7 +3096,7 @@
       </c>
       <c r="E11"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>114</v>
       </c>
@@ -3100,7 +3106,9 @@
       <c r="C12" t="s">
         <v>136</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="E12"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -3623,7 +3631,7 @@
   <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3647,7 +3655,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>78</v>
       </c>
@@ -3658,7 +3666,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -3669,7 +3677,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -3680,7 +3688,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -3691,7 +3699,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>131</v>
       </c>
@@ -3730,7 +3738,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -3741,7 +3749,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -3766,7 +3774,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -3819,7 +3827,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -3830,7 +3838,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>73</v>
       </c>
@@ -3841,7 +3849,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>89</v>
       </c>
@@ -3852,7 +3860,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>97</v>
       </c>
@@ -3863,7 +3871,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>111</v>
       </c>
@@ -3874,7 +3882,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -3927,7 +3935,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -4192,7 +4200,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>39</v>
       </c>
@@ -4201,6 +4209,9 @@
       </c>
       <c r="C45" t="s">
         <v>138</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -4259,7 +4270,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>66</v>
       </c>
@@ -4270,7 +4281,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>98</v>
       </c>
@@ -4281,7 +4292,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>20</v>
       </c>
@@ -4333,7 +4344,7 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="B16" sqref="B16:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4788,7 +4799,7 @@
       </c>
       <c r="E31"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -4797,6 +4808,9 @@
       </c>
       <c r="C32" t="s">
         <v>137</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="E32"/>
     </row>
@@ -4848,7 +4862,7 @@
       </c>
       <c r="E36"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -4857,6 +4871,9 @@
       </c>
       <c r="C37" t="s">
         <v>138</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="E37"/>
     </row>

</xml_diff>

<commit_message>
udte all the things
</commit_message>
<xml_diff>
--- a/divinity/Skills.xlsx
+++ b/divinity/Skills.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jturo\notes\divinity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47F62A9-C273-49F0-843A-B0E8CC0FFAD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D43B8C3-1A6F-4F0A-8BE7-7DC6BD86A372}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{22CF8C86-0986-46F7-901E-B0479304723F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{22CF8C86-0986-46F7-901E-B0479304723F}"/>
   </bookViews>
   <sheets>
     <sheet name="All Skills" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="146">
   <si>
     <t>Aerotheurge</t>
   </si>
@@ -571,8 +571,8 @@
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A48:D107">
-    <sortCondition ref="B1:B129"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D128">
+    <sortCondition ref="A1:A129"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="3" xr3:uid="{C942E722-BCB0-4010-8BDE-D8A787CFEDA6}" name="Skill"/>
@@ -589,11 +589,6 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2567B707-35F9-4175-8E67-C06A8044C0B1}" name="madora" displayName="madora" ref="A1:D23" totalsRowShown="0">
   <autoFilter ref="A1:D23" xr:uid="{BF9C7B15-02F1-4DC6-B7CC-0ADE24FA67EF}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Man-At-Arms"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>
@@ -614,6 +609,11 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{91EF0500-EACC-4F56-8167-B7EC3E2BB0C0}" name="brenda" displayName="brenda" ref="A1:D54" totalsRowShown="0">
   <autoFilter ref="A1:D54" xr:uid="{BF9C7B15-02F1-4DC6-B7CC-0ADE24FA67EF}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Hydrosophist"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>
@@ -636,12 +636,8 @@
   <autoFilter ref="A1:D49" xr:uid="{BF9C7B15-02F1-4DC6-B7CC-0ADE24FA67EF}">
     <filterColumn colId="1">
       <filters>
+        <filter val="Hydrosophist"/>
         <filter val="Witchcraft"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Adept"/>
       </filters>
     </filterColumn>
     <filterColumn colId="3">
@@ -668,11 +664,6 @@
       <filters>
         <filter val="Expert Marksman"/>
         <filter val="Hydrosophist"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Adept"/>
       </filters>
     </filterColumn>
     <filterColumn colId="3">
@@ -991,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E1CE82-3B7C-490C-8774-E0CAC5B9C9EC}">
   <dimension ref="A1:D129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C123" sqref="C123"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,17 +1053,17 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="B5" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D5">
         <f>IF(ISNA(VLOOKUP(A5,danger[],1,FALSE)),0,IF(VLOOKUP(A5,danger[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A5,brenda[],1,FALSE)),0,IF(VLOOKUP(A5,brenda[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A5,madora[],1,FALSE)),0,IF(VLOOKUP(A5,madora[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A5,jehan[],1,FALSE)),0,IF(VLOOKUP(A5,jehan[],4,FALSE)="",1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1182,17 +1173,17 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D13">
         <f>IF(ISNA(VLOOKUP(A13,danger[],1,FALSE)),0,IF(VLOOKUP(A13,danger[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A13,brenda[],1,FALSE)),0,IF(VLOOKUP(A13,brenda[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A13,madora[],1,FALSE)),0,IF(VLOOKUP(A13,madora[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A13,jehan[],1,FALSE)),0,IF(VLOOKUP(A13,jehan[],4,FALSE)="",1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1362,10 +1353,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C25" t="s">
         <v>137</v>
@@ -1422,13 +1413,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D29">
         <f>IF(ISNA(VLOOKUP(A29,danger[],1,FALSE)),0,IF(VLOOKUP(A29,danger[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A29,brenda[],1,FALSE)),0,IF(VLOOKUP(A29,brenda[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A29,madora[],1,FALSE)),0,IF(VLOOKUP(A29,madora[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A29,jehan[],1,FALSE)),0,IF(VLOOKUP(A29,jehan[],4,FALSE)="",1,0))</f>
@@ -1467,10 +1458,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="B32" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C32" t="s">
         <v>137</v>
@@ -1482,32 +1473,32 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="B33" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D33">
         <f>IF(ISNA(VLOOKUP(A33,danger[],1,FALSE)),0,IF(VLOOKUP(A33,danger[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A33,brenda[],1,FALSE)),0,IF(VLOOKUP(A33,brenda[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A33,madora[],1,FALSE)),0,IF(VLOOKUP(A33,madora[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A33,jehan[],1,FALSE)),0,IF(VLOOKUP(A33,jehan[],4,FALSE)="",1,0))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D34">
         <f>IF(ISNA(VLOOKUP(A34,danger[],1,FALSE)),0,IF(VLOOKUP(A34,danger[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A34,brenda[],1,FALSE)),0,IF(VLOOKUP(A34,brenda[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A34,madora[],1,FALSE)),0,IF(VLOOKUP(A34,madora[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A34,jehan[],1,FALSE)),0,IF(VLOOKUP(A34,jehan[],4,FALSE)="",1,0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1797,17 +1788,17 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B54" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C54" t="s">
         <v>137</v>
       </c>
       <c r="D54">
         <f>IF(ISNA(VLOOKUP(A54,danger[],1,FALSE)),0,IF(VLOOKUP(A54,danger[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A54,brenda[],1,FALSE)),0,IF(VLOOKUP(A54,brenda[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A54,madora[],1,FALSE)),0,IF(VLOOKUP(A54,madora[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A54,jehan[],1,FALSE)),0,IF(VLOOKUP(A54,jehan[],4,FALSE)="",1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1857,10 +1848,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="B58" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C58" t="s">
         <v>137</v>
@@ -1902,32 +1893,32 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B61" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C61" t="s">
         <v>137</v>
       </c>
       <c r="D61">
         <f>IF(ISNA(VLOOKUP(A61,danger[],1,FALSE)),0,IF(VLOOKUP(A61,danger[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A61,brenda[],1,FALSE)),0,IF(VLOOKUP(A61,brenda[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A61,madora[],1,FALSE)),0,IF(VLOOKUP(A61,madora[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A61,jehan[],1,FALSE)),0,IF(VLOOKUP(A61,jehan[],4,FALSE)="",1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="B62" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C62" t="s">
         <v>137</v>
       </c>
       <c r="D62">
         <f>IF(ISNA(VLOOKUP(A62,danger[],1,FALSE)),0,IF(VLOOKUP(A62,danger[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A62,brenda[],1,FALSE)),0,IF(VLOOKUP(A62,brenda[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A62,madora[],1,FALSE)),0,IF(VLOOKUP(A62,madora[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A62,jehan[],1,FALSE)),0,IF(VLOOKUP(A62,jehan[],4,FALSE)="",1,0))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1962,13 +1953,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>114</v>
+        <v>20</v>
       </c>
       <c r="B65" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C65" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D65">
         <f>IF(ISNA(VLOOKUP(A65,danger[],1,FALSE)),0,IF(VLOOKUP(A65,danger[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A65,brenda[],1,FALSE)),0,IF(VLOOKUP(A65,brenda[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A65,madora[],1,FALSE)),0,IF(VLOOKUP(A65,madora[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A65,jehan[],1,FALSE)),0,IF(VLOOKUP(A65,jehan[],4,FALSE)="",1,0))</f>
@@ -1992,32 +1983,32 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="B67" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C67" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D67">
         <f>IF(ISNA(VLOOKUP(A67,danger[],1,FALSE)),0,IF(VLOOKUP(A67,danger[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A67,brenda[],1,FALSE)),0,IF(VLOOKUP(A67,brenda[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A67,madora[],1,FALSE)),0,IF(VLOOKUP(A67,madora[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A67,jehan[],1,FALSE)),0,IF(VLOOKUP(A67,jehan[],4,FALSE)="",1,0))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>111</v>
+        <v>39</v>
       </c>
       <c r="B68" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C68" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D68">
         <f>IF(ISNA(VLOOKUP(A68,danger[],1,FALSE)),0,IF(VLOOKUP(A68,danger[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A68,brenda[],1,FALSE)),0,IF(VLOOKUP(A68,brenda[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A68,madora[],1,FALSE)),0,IF(VLOOKUP(A68,madora[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A68,jehan[],1,FALSE)),0,IF(VLOOKUP(A68,jehan[],4,FALSE)="",1,0))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -2097,10 +2088,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B74" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C74" t="s">
         <v>136</v>
@@ -2112,13 +2103,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>135</v>
+        <v>90</v>
       </c>
       <c r="B75" t="s">
         <v>4</v>
       </c>
       <c r="C75" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D75">
         <f>IF(ISNA(VLOOKUP(A75,danger[],1,FALSE)),0,IF(VLOOKUP(A75,danger[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A75,brenda[],1,FALSE)),0,IF(VLOOKUP(A75,brenda[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A75,madora[],1,FALSE)),0,IF(VLOOKUP(A75,madora[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A75,jehan[],1,FALSE)),0,IF(VLOOKUP(A75,jehan[],4,FALSE)="",1,0))</f>
@@ -2172,28 +2163,28 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>40</v>
+        <v>121</v>
       </c>
       <c r="B79" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C79" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D79">
         <f>IF(ISNA(VLOOKUP(A79,danger[],1,FALSE)),0,IF(VLOOKUP(A79,danger[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A79,brenda[],1,FALSE)),0,IF(VLOOKUP(A79,brenda[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A79,madora[],1,FALSE)),0,IF(VLOOKUP(A79,madora[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A79,jehan[],1,FALSE)),0,IF(VLOOKUP(A79,jehan[],4,FALSE)="",1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="B80" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C80" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D80">
         <f>IF(ISNA(VLOOKUP(A80,danger[],1,FALSE)),0,IF(VLOOKUP(A80,danger[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A80,brenda[],1,FALSE)),0,IF(VLOOKUP(A80,brenda[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A80,madora[],1,FALSE)),0,IF(VLOOKUP(A80,madora[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A80,jehan[],1,FALSE)),0,IF(VLOOKUP(A80,jehan[],4,FALSE)="",1,0))</f>
@@ -2217,7 +2208,7 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="B82" t="s">
         <v>0</v>
@@ -2227,7 +2218,7 @@
       </c>
       <c r="D82">
         <f>IF(ISNA(VLOOKUP(A82,danger[],1,FALSE)),0,IF(VLOOKUP(A82,danger[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A82,brenda[],1,FALSE)),0,IF(VLOOKUP(A82,brenda[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A82,madora[],1,FALSE)),0,IF(VLOOKUP(A82,madora[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A82,jehan[],1,FALSE)),0,IF(VLOOKUP(A82,jehan[],4,FALSE)="",1,0))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -2427,13 +2418,13 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>113</v>
+        <v>43</v>
       </c>
       <c r="B96" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C96" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D96">
         <f>IF(ISNA(VLOOKUP(A96,danger[],1,FALSE)),0,IF(VLOOKUP(A96,danger[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A96,brenda[],1,FALSE)),0,IF(VLOOKUP(A96,brenda[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A96,madora[],1,FALSE)),0,IF(VLOOKUP(A96,madora[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A96,jehan[],1,FALSE)),0,IF(VLOOKUP(A96,jehan[],4,FALSE)="",1,0))</f>
@@ -2442,17 +2433,17 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>11</v>
+        <v>135</v>
       </c>
       <c r="B97" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C97" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D97">
         <f>IF(ISNA(VLOOKUP(A97,danger[],1,FALSE)),0,IF(VLOOKUP(A97,danger[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A97,brenda[],1,FALSE)),0,IF(VLOOKUP(A97,brenda[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A97,madora[],1,FALSE)),0,IF(VLOOKUP(A97,madora[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A97,jehan[],1,FALSE)),0,IF(VLOOKUP(A97,jehan[],4,FALSE)="",1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -2502,17 +2493,17 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>43</v>
+        <v>98</v>
       </c>
       <c r="B101" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C101" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D101">
         <f>IF(ISNA(VLOOKUP(A101,danger[],1,FALSE)),0,IF(VLOOKUP(A101,danger[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A101,brenda[],1,FALSE)),0,IF(VLOOKUP(A101,brenda[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A101,madora[],1,FALSE)),0,IF(VLOOKUP(A101,madora[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A101,jehan[],1,FALSE)),0,IF(VLOOKUP(A101,jehan[],4,FALSE)="",1,0))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -2562,17 +2553,17 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="B105" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C105" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D105">
         <f>IF(ISNA(VLOOKUP(A105,danger[],1,FALSE)),0,IF(VLOOKUP(A105,danger[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A105,brenda[],1,FALSE)),0,IF(VLOOKUP(A105,brenda[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A105,madora[],1,FALSE)),0,IF(VLOOKUP(A105,madora[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A105,jehan[],1,FALSE)),0,IF(VLOOKUP(A105,jehan[],4,FALSE)="",1,0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -2772,10 +2763,10 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B119" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C119" t="s">
         <v>138</v>
@@ -2802,17 +2793,17 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B121" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C121" t="s">
         <v>138</v>
       </c>
       <c r="D121">
         <f>IF(ISNA(VLOOKUP(A121,danger[],1,FALSE)),0,IF(VLOOKUP(A121,danger[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A121,brenda[],1,FALSE)),0,IF(VLOOKUP(A121,brenda[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A121,madora[],1,FALSE)),0,IF(VLOOKUP(A121,madora[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A121,jehan[],1,FALSE)),0,IF(VLOOKUP(A121,jehan[],4,FALSE)="",1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -2832,13 +2823,13 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>12</v>
+        <v>106</v>
       </c>
       <c r="B123" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C123" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D123">
         <f>IF(ISNA(VLOOKUP(A123,danger[],1,FALSE)),0,IF(VLOOKUP(A123,danger[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A123,brenda[],1,FALSE)),0,IF(VLOOKUP(A123,brenda[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A123,madora[],1,FALSE)),0,IF(VLOOKUP(A123,madora[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A123,jehan[],1,FALSE)),0,IF(VLOOKUP(A123,jehan[],4,FALSE)="",1,0))</f>
@@ -2847,17 +2838,17 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="B124" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C124" t="s">
         <v>138</v>
       </c>
       <c r="D124">
         <f>IF(ISNA(VLOOKUP(A124,danger[],1,FALSE)),0,IF(VLOOKUP(A124,danger[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A124,brenda[],1,FALSE)),0,IF(VLOOKUP(A124,brenda[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A124,madora[],1,FALSE)),0,IF(VLOOKUP(A124,madora[],4,FALSE)="",1,0))+IF(ISNA(VLOOKUP(A124,jehan[],1,FALSE)),0,IF(VLOOKUP(A124,jehan[],4,FALSE)="",1,0))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -2907,10 +2898,10 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B128" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C128" t="s">
         <v>138</v>
@@ -2948,7 +2939,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3139,7 +3130,7 @@
       </c>
       <c r="E12"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>121</v>
       </c>
@@ -3148,6 +3139,9 @@
       </c>
       <c r="C13" t="s">
         <v>136</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="E13"/>
     </row>
@@ -3241,7 +3235,7 @@
       </c>
       <c r="E19"/>
     </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -3311,7 +3305,7 @@
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3336,7 +3330,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>78</v>
       </c>
@@ -3347,7 +3341,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -3358,7 +3352,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -3372,7 +3366,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -3383,7 +3377,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>131</v>
       </c>
@@ -3422,7 +3416,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -3433,7 +3427,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -3458,7 +3452,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -3838,7 +3832,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>85</v>
       </c>
@@ -3863,7 +3857,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -4280,7 +4274,7 @@
       </c>
       <c r="E15"/>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -4322,7 +4316,7 @@
       </c>
       <c r="E18"/>
     </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>89</v>
       </c>
@@ -4334,7 +4328,7 @@
       </c>
       <c r="E19"/>
     </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>111</v>
       </c>
@@ -4361,7 +4355,7 @@
       </c>
       <c r="E21"/>
     </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>97</v>
       </c>
@@ -4778,7 +4772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F3251A-F89B-4FD0-9CE0-048C986F7283}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
@@ -4969,7 +4963,7 @@
       </c>
       <c r="E12"/>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>122</v>
       </c>
@@ -5008,7 +5002,7 @@
       <c r="D15" s="1"/>
       <c r="E15"/>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>111</v>
       </c>

</xml_diff>